<commit_message>
add line chart of population transition
</commit_message>
<xml_diff>
--- a/data/kanagawa_jinkou.xlsx
+++ b/data/kanagawa_jinkou.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18645" windowHeight="9570" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18645" windowHeight="9570" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="市町村一覧" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="316">
   <si>
     <t>市　町　村　一　覧</t>
   </si>
@@ -709,6 +709,45 @@
   </si>
   <si>
     <t>小田原市、南足柄市、中井町、大井町、松田町、山北町、開成町、箱根町、真鶴町、湯河原町</t>
+  </si>
+  <si>
+    <t>県人口推移（月次）</t>
+  </si>
+  <si>
+    <t>1月</t>
+  </si>
+  <si>
+    <t>2月</t>
+  </si>
+  <si>
+    <t>3月</t>
+  </si>
+  <si>
+    <t>4月</t>
+  </si>
+  <si>
+    <t>5月</t>
+  </si>
+  <si>
+    <t>6月</t>
+  </si>
+  <si>
+    <t>7月</t>
+  </si>
+  <si>
+    <t>8月</t>
+  </si>
+  <si>
+    <t>9月</t>
+  </si>
+  <si>
+    <t>10月</t>
+  </si>
+  <si>
+    <t>11月</t>
+  </si>
+  <si>
+    <t>12月</t>
   </si>
   <si>
     <t>2018年</t>
@@ -2218,16 +2257,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="11">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="[$-411]#,##0;\-#,##0"/>
+    <numFmt numFmtId="182" formatCode="#,##0_ "/>
+    <numFmt numFmtId="183" formatCode="\+0.00%;\-0.00%;"/>
+    <numFmt numFmtId="184" formatCode="\+#,##0;\-#,##0;"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-411]#,##0;\-#,##0"/>
-    <numFmt numFmtId="178" formatCode="#,##0_ "/>
-    <numFmt numFmtId="179" formatCode="0_ "/>
-    <numFmt numFmtId="180" formatCode="\+0.00%;\-0.00%;"/>
-    <numFmt numFmtId="181" formatCode="\+#,##0;\-#,##0;"/>
-    <numFmt numFmtId="182" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="183" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="184" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="51">
@@ -2394,93 +2433,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2498,23 +2460,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2536,9 +2491,93 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2594,7 +2633,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2606,13 +2657,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2624,7 +2735,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2636,19 +2747,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2661,6 +2784,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2679,96 +2808,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3387,32 +3426,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3426,11 +3444,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3450,6 +3474,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -3459,30 +3498,30 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3494,79 +3533,76 @@
     <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="53" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="37" borderId="58" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="36" borderId="58" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="54" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="34" borderId="55" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="34" borderId="56" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="18" borderId="56" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="55" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="32" borderId="56" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="32" borderId="55" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="52" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3575,54 +3611,57 @@
     <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="181" fontId="50" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -3708,13 +3747,13 @@
     <xf numFmtId="37" fontId="12" fillId="2" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="2" borderId="13" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="13" fillId="2" borderId="13" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="2" borderId="17" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="13" fillId="2" borderId="17" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="2" borderId="18" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="13" fillId="2" borderId="18" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="12" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3726,25 +3765,25 @@
     <xf numFmtId="37" fontId="15" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="13" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="13" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="17" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="17" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="18" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="18" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="15" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="13" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="13" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="17" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="17" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="18" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="18" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="1" fillId="3" borderId="12" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3756,13 +3795,13 @@
     <xf numFmtId="37" fontId="15" fillId="3" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="13" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="3" borderId="13" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="17" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="3" borderId="17" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="18" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="3" borderId="18" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="16" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3828,29 +3867,29 @@
     <xf numFmtId="37" fontId="8" fillId="0" borderId="26" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="183" fontId="13" fillId="2" borderId="27" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="13" fillId="2" borderId="27" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="2" borderId="28" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="13" fillId="2" borderId="28" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="183" fontId="2" fillId="0" borderId="27" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="27" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="28" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="28" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="15" fillId="0" borderId="27" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="27" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="28" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="28" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="2" fillId="3" borderId="27" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="27" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="28" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="3" borderId="28" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3872,42 +3911,42 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="21" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="21" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="21" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="21" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" xfId="49" applyFont="1"/>
-    <xf numFmtId="177" fontId="23" fillId="0" borderId="34" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="181" fontId="23" fillId="0" borderId="34" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="11" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="11" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="14" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="14" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="24" fillId="4" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="24" fillId="4" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="5" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="22" fillId="5" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="6" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="22" fillId="6" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="16" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="17" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="5" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="16" fillId="5" borderId="0" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3928,17 +3967,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="34" xfId="49" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="34" xfId="49" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="12" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3947,7 +3989,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3956,66 +3998,66 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="2" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="13" fillId="2" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="2" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="13" fillId="2" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="2" fillId="3" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="34" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="34" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -7270,7 +7312,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>県人口推移!$B$1</c:f>
+              <c:f>県人口推移!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7339,53 +7381,52 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>県人口推移!$A$2:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>県人口推移!$A$9:$A$20</c:f>
+              <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1月</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2月</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3月</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4月</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>5月</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>6月</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>7月</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>8月</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>9月</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>10月</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>11月</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>県人口推移!$B$2:$B$13</c:f>
+              <c:f>県人口推移!$B$9:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -7435,7 +7476,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>県人口推移!$C$1</c:f>
+              <c:f>県人口推移!$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7504,53 +7545,52 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>県人口推移!$A$2:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>県人口推移!$A$9:$A$20</c:f>
+              <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1月</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2月</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3月</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4月</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>5月</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>6月</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>7月</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>8月</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>9月</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>10月</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>11月</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>県人口推移!$C$2:$C$13</c:f>
+              <c:f>県人口推移!$C$9:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -7600,7 +7640,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>県人口推移!$D$1</c:f>
+              <c:f>県人口推移!$D$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7669,53 +7709,52 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>県人口推移!$A$2:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>県人口推移!$A$9:$A$20</c:f>
+              <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1月</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2月</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3月</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4月</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>5月</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>6月</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>7月</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>8月</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>9月</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>10月</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>11月</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>12月</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>県人口推移!$D$2:$D$13</c:f>
+              <c:f>県人口推移!$D$9:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -11493,13 +11532,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>314280</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>142920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>256680</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -11508,7 +11547,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4171315" y="561975"/>
+        <a:off x="4171315" y="2028825"/>
         <a:ext cx="4572000" cy="3552190"/>
       </xdr:xfrm>
       <a:graphic>
@@ -11989,55 +12028,55 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20" style="142" customWidth="1"/>
-    <col min="2" max="2" width="12.4285714285714" style="145" customWidth="1"/>
-    <col min="3" max="3" width="40.5714285714286" style="145" customWidth="1"/>
-    <col min="4" max="4" width="19" style="146" customWidth="1"/>
-    <col min="5" max="5" width="49.5714285714286" style="145" customWidth="1"/>
-    <col min="6" max="6" width="14.4285714285714" style="145" customWidth="1"/>
-    <col min="7" max="7" width="20" style="142" customWidth="1"/>
-    <col min="8" max="8" width="14.4285714285714" style="145" customWidth="1"/>
-    <col min="9" max="9" width="21.2857142857143" style="142" customWidth="1"/>
-    <col min="10" max="11" width="18.5714285714286" style="145" customWidth="1"/>
-    <col min="12" max="16384" width="10.2857142857143" style="145"/>
+    <col min="1" max="1" width="20" style="143" customWidth="1"/>
+    <col min="2" max="2" width="12.4285714285714" style="146" customWidth="1"/>
+    <col min="3" max="3" width="40.5714285714286" style="146" customWidth="1"/>
+    <col min="4" max="4" width="19" style="147" customWidth="1"/>
+    <col min="5" max="5" width="49.5714285714286" style="146" customWidth="1"/>
+    <col min="6" max="6" width="14.4285714285714" style="146" customWidth="1"/>
+    <col min="7" max="7" width="20" style="143" customWidth="1"/>
+    <col min="8" max="8" width="14.4285714285714" style="146" customWidth="1"/>
+    <col min="9" max="9" width="21.2857142857143" style="143" customWidth="1"/>
+    <col min="10" max="11" width="18.5714285714286" style="146" customWidth="1"/>
+    <col min="12" max="16384" width="10.2857142857143" style="146"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="147" t="s">
+      <c r="G1" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="145"/>
+      <c r="I1" s="146"/>
     </row>
     <row r="2" ht="4.5" customHeight="1"/>
-    <row r="3" s="142" customFormat="1" ht="18" customHeight="1" spans="1:11">
-      <c r="A3" s="120" t="s">
+    <row r="3" s="143" customFormat="1" ht="18" customHeight="1" spans="1:11">
+      <c r="A3" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="150" t="s">
+      <c r="D3" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="151" t="s">
+      <c r="E3" s="152" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="120" t="s">
+      <c r="G3" s="121" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="120" t="s">
+      <c r="I3" s="121" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="10" t="s">
@@ -12051,16 +12090,16 @@
       <c r="A4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="152" t="s">
+      <c r="B4" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="154" t="s">
+      <c r="D4" s="155" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="155" t="s">
+      <c r="E4" s="156" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="26">
@@ -12086,16 +12125,16 @@
       <c r="A5" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="156" t="s">
+      <c r="B5" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="158" t="s">
+      <c r="D5" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="155" t="s">
+      <c r="E5" s="156" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="53">
@@ -12119,16 +12158,16 @@
       <c r="A6" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="158" t="s">
+      <c r="D6" s="159" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="159" t="s">
+      <c r="E6" s="160" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="53">
@@ -12152,16 +12191,16 @@
       <c r="A7" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="156" t="s">
+      <c r="B7" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="157" t="s">
+      <c r="C7" s="158" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="158" t="s">
+      <c r="D7" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="159" t="s">
+      <c r="E7" s="160" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="53">
@@ -12185,16 +12224,16 @@
       <c r="A8" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="156" t="s">
+      <c r="B8" s="157" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="157" t="s">
+      <c r="C8" s="158" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="158" t="s">
+      <c r="D8" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="155" t="s">
+      <c r="E8" s="156" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="53">
@@ -12214,20 +12253,20 @@
       </c>
       <c r="K8" s="53"/>
     </row>
-    <row r="9" s="143" customFormat="1" customHeight="1" spans="1:11">
+    <row r="9" s="144" customFormat="1" customHeight="1" spans="1:11">
       <c r="A9" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="160" t="s">
+      <c r="B9" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="157" t="s">
+      <c r="C9" s="158" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="161" t="s">
+      <c r="D9" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="162" t="s">
+      <c r="E9" s="163" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="53">
@@ -12251,16 +12290,16 @@
       <c r="A10" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="156" t="s">
+      <c r="B10" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="163" t="s">
+      <c r="C10" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="158" t="s">
+      <c r="D10" s="159" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="159" t="s">
+      <c r="E10" s="160" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="53">
@@ -12284,16 +12323,16 @@
       <c r="A11" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="156" t="s">
+      <c r="B11" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="157" t="s">
+      <c r="C11" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="158" t="s">
+      <c r="D11" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="159" t="s">
+      <c r="E11" s="160" t="s">
         <v>54</v>
       </c>
       <c r="F11" s="53">
@@ -12317,16 +12356,16 @@
       <c r="A12" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="160" t="s">
+      <c r="B12" s="161" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="157" t="s">
+      <c r="C12" s="158" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="161" t="s">
+      <c r="D12" s="162" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="162" t="s">
+      <c r="E12" s="163" t="s">
         <v>60</v>
       </c>
       <c r="F12" s="53">
@@ -12350,16 +12389,16 @@
       <c r="A13" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="157" t="s">
+      <c r="C13" s="158" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="158" t="s">
+      <c r="D13" s="159" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="159" t="s">
+      <c r="E13" s="160" t="s">
         <v>65</v>
       </c>
       <c r="F13" s="53">
@@ -12383,16 +12422,16 @@
       <c r="A14" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="165" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="157" t="s">
+      <c r="C14" s="158" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="165" t="s">
+      <c r="D14" s="166" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="155" t="s">
+      <c r="E14" s="156" t="s">
         <v>70</v>
       </c>
       <c r="F14" s="53">
@@ -12416,16 +12455,16 @@
       <c r="A15" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="157" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="157" t="s">
+      <c r="C15" s="158" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="158" t="s">
+      <c r="D15" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="159" t="s">
+      <c r="E15" s="160" t="s">
         <v>75</v>
       </c>
       <c r="F15" s="53">
@@ -12449,16 +12488,16 @@
       <c r="A16" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="157" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="157" t="s">
+      <c r="C16" s="158" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="158" t="s">
+      <c r="D16" s="159" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="159" t="s">
+      <c r="E16" s="160" t="s">
         <v>80</v>
       </c>
       <c r="F16" s="53">
@@ -12482,16 +12521,16 @@
       <c r="A17" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="156" t="s">
+      <c r="B17" s="157" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="157" t="s">
+      <c r="C17" s="158" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="158" t="s">
+      <c r="D17" s="159" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="166" t="s">
+      <c r="E17" s="167" t="s">
         <v>85</v>
       </c>
       <c r="F17" s="53">
@@ -12515,16 +12554,16 @@
       <c r="A18" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="156" t="s">
+      <c r="B18" s="157" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="157" t="s">
+      <c r="C18" s="158" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="158" t="s">
+      <c r="D18" s="159" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="162" t="s">
+      <c r="E18" s="163" t="s">
         <v>90</v>
       </c>
       <c r="F18" s="53">
@@ -12548,16 +12587,16 @@
       <c r="A19" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="156" t="s">
+      <c r="B19" s="157" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="157" t="s">
+      <c r="C19" s="158" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="158" t="s">
+      <c r="D19" s="159" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="159" t="s">
+      <c r="E19" s="160" t="s">
         <v>95</v>
       </c>
       <c r="F19" s="53">
@@ -12581,16 +12620,16 @@
       <c r="A20" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="156" t="s">
+      <c r="B20" s="157" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="157" t="s">
+      <c r="C20" s="158" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="158" t="s">
+      <c r="D20" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="159" t="s">
+      <c r="E20" s="160" t="s">
         <v>100</v>
       </c>
       <c r="F20" s="53">
@@ -12614,16 +12653,16 @@
       <c r="A21" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="156" t="s">
+      <c r="B21" s="157" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="163" t="s">
+      <c r="C21" s="164" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="158" t="s">
+      <c r="D21" s="159" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="155" t="s">
+      <c r="E21" s="156" t="s">
         <v>105</v>
       </c>
       <c r="F21" s="53">
@@ -12647,16 +12686,16 @@
       <c r="A22" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="156" t="s">
+      <c r="B22" s="157" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="163" t="s">
+      <c r="C22" s="164" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="158" t="s">
+      <c r="D22" s="159" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="159" t="s">
+      <c r="E22" s="160" t="s">
         <v>110</v>
       </c>
       <c r="F22" s="53">
@@ -12680,16 +12719,16 @@
       <c r="A23" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="156" t="s">
+      <c r="B23" s="157" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="157" t="s">
+      <c r="C23" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="158" t="s">
+      <c r="D23" s="159" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="159" t="s">
+      <c r="E23" s="160" t="s">
         <v>115</v>
       </c>
       <c r="F23" s="53">
@@ -12713,16 +12752,16 @@
       <c r="A24" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="156" t="s">
+      <c r="B24" s="157" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="163" t="s">
+      <c r="C24" s="164" t="s">
         <v>118</v>
       </c>
-      <c r="D24" s="158" t="s">
+      <c r="D24" s="159" t="s">
         <v>119</v>
       </c>
-      <c r="E24" s="159" t="s">
+      <c r="E24" s="160" t="s">
         <v>120</v>
       </c>
       <c r="F24" s="53">
@@ -12746,16 +12785,16 @@
       <c r="A25" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="B25" s="156" t="s">
+      <c r="B25" s="157" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="157" t="s">
+      <c r="C25" s="158" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="158" t="s">
+      <c r="D25" s="159" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="167" t="s">
+      <c r="E25" s="168" t="s">
         <v>125</v>
       </c>
       <c r="F25" s="53">
@@ -12779,16 +12818,16 @@
       <c r="A26" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="156" t="s">
+      <c r="B26" s="157" t="s">
         <v>127</v>
       </c>
-      <c r="C26" s="157" t="s">
+      <c r="C26" s="158" t="s">
         <v>128</v>
       </c>
-      <c r="D26" s="158" t="s">
+      <c r="D26" s="159" t="s">
         <v>129</v>
       </c>
-      <c r="E26" s="168" t="s">
+      <c r="E26" s="169" t="s">
         <v>130</v>
       </c>
       <c r="F26" s="53">
@@ -12812,16 +12851,16 @@
       <c r="A27" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="156" t="s">
+      <c r="B27" s="157" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="163" t="s">
+      <c r="C27" s="164" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="158" t="s">
+      <c r="D27" s="159" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="159" t="s">
+      <c r="E27" s="160" t="s">
         <v>135</v>
       </c>
       <c r="F27" s="53">
@@ -12845,16 +12884,16 @@
       <c r="A28" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="156" t="s">
+      <c r="B28" s="157" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="157" t="s">
+      <c r="C28" s="158" t="s">
         <v>138</v>
       </c>
-      <c r="D28" s="158" t="s">
+      <c r="D28" s="159" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="155" t="s">
+      <c r="E28" s="156" t="s">
         <v>140</v>
       </c>
       <c r="F28" s="53">
@@ -12878,16 +12917,16 @@
       <c r="A29" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="B29" s="156" t="s">
+      <c r="B29" s="157" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="157" t="s">
+      <c r="C29" s="158" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="158" t="s">
+      <c r="D29" s="159" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="159" t="s">
+      <c r="E29" s="160" t="s">
         <v>145</v>
       </c>
       <c r="F29" s="53">
@@ -12911,16 +12950,16 @@
       <c r="A30" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="156" t="s">
+      <c r="B30" s="157" t="s">
         <v>147</v>
       </c>
-      <c r="C30" s="163" t="s">
+      <c r="C30" s="164" t="s">
         <v>148</v>
       </c>
-      <c r="D30" s="158" t="s">
+      <c r="D30" s="159" t="s">
         <v>149</v>
       </c>
-      <c r="E30" s="159" t="s">
+      <c r="E30" s="160" t="s">
         <v>150</v>
       </c>
       <c r="F30" s="53">
@@ -12944,16 +12983,16 @@
       <c r="A31" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="156" t="s">
+      <c r="B31" s="157" t="s">
         <v>152</v>
       </c>
-      <c r="C31" s="163" t="s">
+      <c r="C31" s="164" t="s">
         <v>153</v>
       </c>
-      <c r="D31" s="158" t="s">
+      <c r="D31" s="159" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="159" t="s">
+      <c r="E31" s="160" t="s">
         <v>155</v>
       </c>
       <c r="F31" s="53">
@@ -12977,16 +13016,16 @@
       <c r="A32" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="156" t="s">
+      <c r="B32" s="157" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="163" t="s">
+      <c r="C32" s="164" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="169" t="s">
+      <c r="D32" s="170" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="159" t="s">
+      <c r="E32" s="160" t="s">
         <v>160</v>
       </c>
       <c r="F32" s="53">
@@ -13010,16 +13049,16 @@
       <c r="A33" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="156" t="s">
+      <c r="B33" s="157" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="163" t="s">
+      <c r="C33" s="164" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="158" t="s">
+      <c r="D33" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="159" t="s">
+      <c r="E33" s="160" t="s">
         <v>165</v>
       </c>
       <c r="F33" s="53">
@@ -13043,16 +13082,16 @@
       <c r="A34" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="B34" s="156" t="s">
+      <c r="B34" s="157" t="s">
         <v>167</v>
       </c>
-      <c r="C34" s="157" t="s">
+      <c r="C34" s="158" t="s">
         <v>168</v>
       </c>
-      <c r="D34" s="158" t="s">
+      <c r="D34" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="159" t="s">
+      <c r="E34" s="160" t="s">
         <v>170</v>
       </c>
       <c r="F34" s="53">
@@ -13072,20 +13111,20 @@
       </c>
       <c r="K34" s="53"/>
     </row>
-    <row r="35" s="144" customFormat="1" customHeight="1" spans="1:11">
+    <row r="35" s="145" customFormat="1" customHeight="1" spans="1:11">
       <c r="A35" s="81" t="s">
         <v>171</v>
       </c>
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="165" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="157" t="s">
+      <c r="C35" s="158" t="s">
         <v>173</v>
       </c>
-      <c r="D35" s="165" t="s">
+      <c r="D35" s="166" t="s">
         <v>174</v>
       </c>
-      <c r="E35" s="170" t="s">
+      <c r="E35" s="171" t="s">
         <v>175</v>
       </c>
       <c r="F35" s="53">
@@ -13109,16 +13148,16 @@
       <c r="A36" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="B36" s="171" t="s">
+      <c r="B36" s="172" t="s">
         <v>177</v>
       </c>
-      <c r="C36" s="172" t="s">
+      <c r="C36" s="173" t="s">
         <v>178</v>
       </c>
-      <c r="D36" s="173" t="s">
+      <c r="D36" s="174" t="s">
         <v>179</v>
       </c>
-      <c r="E36" s="174" t="s">
+      <c r="E36" s="175" t="s">
         <v>180</v>
       </c>
       <c r="F36" s="82">
@@ -13139,15 +13178,15 @@
       <c r="K36" s="82"/>
     </row>
     <row r="37" ht="20.25" customHeight="1" spans="2:11">
-      <c r="B37" s="175"/>
-      <c r="C37" s="145" t="s">
+      <c r="B37" s="176"/>
+      <c r="C37" s="146" t="s">
         <v>181</v>
       </c>
-      <c r="E37" s="176"/>
-      <c r="F37" s="177"/>
-      <c r="H37" s="177"/>
-      <c r="J37" s="177"/>
-      <c r="K37" s="177"/>
+      <c r="E37" s="177"/>
+      <c r="F37" s="178"/>
+      <c r="H37" s="178"/>
+      <c r="J37" s="178"/>
+      <c r="K37" s="178"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -13197,7 +13236,7 @@
   <sheetPr/>
   <dimension ref="B1:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F43" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="F43" workbookViewId="0">
       <selection activeCell="L51" sqref="L51:L56"/>
     </sheetView>
   </sheetViews>
@@ -13262,24 +13301,24 @@
       <c r="D3" s="94" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="114"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="114"/>
-      <c r="U3" s="114"/>
-      <c r="V3" s="141" t="s">
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
+      <c r="Q3" s="115"/>
+      <c r="R3" s="115"/>
+      <c r="S3" s="115"/>
+      <c r="T3" s="115"/>
+      <c r="U3" s="115"/>
+      <c r="V3" s="142" t="s">
         <v>184</v>
       </c>
     </row>
@@ -13288,7 +13327,7 @@
       <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="115"/>
+      <c r="E6" s="116"/>
       <c r="F6" s="95" t="s">
         <v>185</v>
       </c>
@@ -13298,26 +13337,26 @@
       <c r="H6" s="95" t="s">
         <v>187</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="120"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="121"/>
       <c r="K6" s="10" t="s">
         <v>8</v>
       </c>
       <c r="L6" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="M6" s="121" t="s">
+      <c r="M6" s="122" t="s">
         <v>188</v>
       </c>
-      <c r="N6" s="121" t="s">
+      <c r="N6" s="122" t="s">
         <v>189</v>
       </c>
-      <c r="O6" s="119"/>
-      <c r="P6" s="119"/>
-      <c r="Q6" s="119"/>
+      <c r="O6" s="120"/>
+      <c r="P6" s="120"/>
+      <c r="Q6" s="120"/>
     </row>
     <row r="7" spans="5:17">
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="117" t="s">
         <v>190</v>
       </c>
       <c r="F7" s="96" t="s">
@@ -13329,21 +13368,21 @@
       <c r="H7" s="96" t="s">
         <v>191</v>
       </c>
-      <c r="I7" s="122"/>
-      <c r="J7" s="122"/>
-      <c r="K7" s="122"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
       <c r="L7" s="96" t="s">
         <v>191</v>
       </c>
-      <c r="M7" s="122" t="s">
+      <c r="M7" s="123" t="s">
         <v>192</v>
       </c>
-      <c r="N7" s="122" t="s">
+      <c r="N7" s="123" t="s">
         <v>193</v>
       </c>
-      <c r="O7" s="122"/>
-      <c r="P7" s="122"/>
-      <c r="Q7" s="122"/>
+      <c r="O7" s="123"/>
+      <c r="P7" s="123"/>
+      <c r="Q7" s="123"/>
     </row>
     <row r="8" ht="18.75" spans="3:17">
       <c r="C8">
@@ -13364,23 +13403,23 @@
       <c r="H8" s="33">
         <v>4625940</v>
       </c>
-      <c r="I8" s="123"/>
-      <c r="J8" s="123"/>
-      <c r="K8" s="123"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
       <c r="L8" s="32">
         <v>9222618</v>
       </c>
-      <c r="M8" s="124">
+      <c r="M8" s="125">
         <f>SUM(M12:M44)</f>
         <v>2416.36</v>
       </c>
-      <c r="N8" s="124">
+      <c r="N8" s="125">
         <f>L8/M8</f>
         <v>3816.74005528977</v>
       </c>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="123"/>
+      <c r="O8" s="124"/>
+      <c r="P8" s="124"/>
+      <c r="Q8" s="124"/>
     </row>
     <row r="9" ht="18.75" spans="4:17">
       <c r="D9" s="98" t="s">
@@ -13398,17 +13437,17 @@
       <c r="H9" s="39">
         <v>4480053</v>
       </c>
-      <c r="I9" s="125"/>
-      <c r="J9" s="125"/>
-      <c r="K9" s="125"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="126"/>
+      <c r="K9" s="126"/>
       <c r="L9" s="38">
         <v>8935302</v>
       </c>
-      <c r="M9" s="126"/>
-      <c r="N9" s="126"/>
-      <c r="O9" s="125"/>
-      <c r="P9" s="125"/>
-      <c r="Q9" s="125"/>
+      <c r="M9" s="127"/>
+      <c r="N9" s="127"/>
+      <c r="O9" s="126"/>
+      <c r="P9" s="126"/>
+      <c r="Q9" s="126"/>
     </row>
     <row r="10" ht="18.75" spans="4:17">
       <c r="D10" s="99" t="s">
@@ -13426,21 +13465,21 @@
       <c r="H10" s="39">
         <v>145887</v>
       </c>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
-      <c r="K10" s="125"/>
+      <c r="I10" s="126"/>
+      <c r="J10" s="126"/>
+      <c r="K10" s="126"/>
       <c r="L10" s="38">
         <v>287316</v>
       </c>
-      <c r="M10" s="126"/>
-      <c r="N10" s="126"/>
-      <c r="O10" s="125"/>
-      <c r="P10" s="125"/>
-      <c r="Q10" s="125"/>
+      <c r="M10" s="127"/>
+      <c r="N10" s="127"/>
+      <c r="O10" s="126"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="126"/>
     </row>
     <row r="11" spans="13:14">
-      <c r="M11" s="127"/>
-      <c r="N11" s="127"/>
+      <c r="M11" s="128"/>
+      <c r="N11" s="128"/>
     </row>
     <row r="12" ht="18.75" spans="2:17">
       <c r="B12">
@@ -13464,7 +13503,7 @@
       <c r="H12" s="49">
         <v>1892418</v>
       </c>
-      <c r="I12" s="128"/>
+      <c r="I12" s="129"/>
       <c r="J12" s="27"/>
       <c r="K12" s="26" t="s">
         <v>15</v>
@@ -13472,16 +13511,16 @@
       <c r="L12" s="48">
         <v>3760467</v>
       </c>
-      <c r="M12" s="129">
+      <c r="M12" s="130">
         <v>437.56</v>
       </c>
-      <c r="N12" s="130">
+      <c r="N12" s="131">
         <f t="shared" ref="N12:N44" si="0">L12/M12</f>
         <v>8594.17451320962</v>
       </c>
-      <c r="O12" s="128"/>
-      <c r="P12" s="128"/>
-      <c r="Q12" s="128"/>
+      <c r="O12" s="129"/>
+      <c r="P12" s="129"/>
+      <c r="Q12" s="129"/>
     </row>
     <row r="13" ht="18.75" spans="2:17">
       <c r="B13">
@@ -13505,7 +13544,7 @@
       <c r="H13" s="49">
         <v>760923</v>
       </c>
-      <c r="I13" s="128"/>
+      <c r="I13" s="129"/>
       <c r="J13" s="54"/>
       <c r="K13" s="53" t="s">
         <v>21</v>
@@ -13513,16 +13552,16 @@
       <c r="L13" s="48">
         <v>1539284</v>
       </c>
-      <c r="M13" s="131">
+      <c r="M13" s="132">
         <v>143.01</v>
       </c>
-      <c r="N13" s="132">
+      <c r="N13" s="133">
         <f t="shared" si="0"/>
         <v>10763.471085938</v>
       </c>
-      <c r="O13" s="128"/>
-      <c r="P13" s="128"/>
-      <c r="Q13" s="128"/>
+      <c r="O13" s="129"/>
+      <c r="P13" s="129"/>
+      <c r="Q13" s="129"/>
     </row>
     <row r="14" ht="18.75" spans="2:17">
       <c r="B14">
@@ -13546,7 +13585,7 @@
       <c r="H14" s="49">
         <v>361811</v>
       </c>
-      <c r="I14" s="128"/>
+      <c r="I14" s="129"/>
       <c r="J14" s="54"/>
       <c r="K14" s="53" t="s">
         <v>27</v>
@@ -13554,16 +13593,16 @@
       <c r="L14" s="48">
         <v>723197</v>
       </c>
-      <c r="M14" s="131">
+      <c r="M14" s="132">
         <v>328.91</v>
       </c>
-      <c r="N14" s="132">
+      <c r="N14" s="133">
         <f t="shared" si="0"/>
         <v>2198.76866011979</v>
       </c>
-      <c r="O14" s="128"/>
-      <c r="P14" s="128"/>
-      <c r="Q14" s="128"/>
+      <c r="O14" s="129"/>
+      <c r="P14" s="129"/>
+      <c r="Q14" s="129"/>
     </row>
     <row r="15" spans="2:17">
       <c r="B15">
@@ -13587,7 +13626,7 @@
       <c r="H15" s="39">
         <v>196296</v>
       </c>
-      <c r="I15" s="125"/>
+      <c r="I15" s="126"/>
       <c r="J15" s="54"/>
       <c r="K15" s="53" t="s">
         <v>33</v>
@@ -13595,16 +13634,16 @@
       <c r="L15" s="38">
         <v>393147</v>
       </c>
-      <c r="M15" s="131">
+      <c r="M15" s="132">
         <v>100.82</v>
       </c>
-      <c r="N15" s="132">
+      <c r="N15" s="133">
         <f t="shared" si="0"/>
         <v>3899.49414798651</v>
       </c>
-      <c r="O15" s="125"/>
-      <c r="P15" s="125"/>
-      <c r="Q15" s="125"/>
+      <c r="O15" s="126"/>
+      <c r="P15" s="126"/>
+      <c r="Q15" s="126"/>
     </row>
     <row r="16" spans="2:17">
       <c r="B16">
@@ -13628,7 +13667,7 @@
       <c r="H16" s="39">
         <v>128704</v>
       </c>
-      <c r="I16" s="125"/>
+      <c r="I16" s="126"/>
       <c r="J16" s="54"/>
       <c r="K16" s="53" t="s">
         <v>39</v>
@@ -13636,16 +13675,16 @@
       <c r="L16" s="38">
         <v>257670</v>
       </c>
-      <c r="M16" s="131">
+      <c r="M16" s="132">
         <v>67.88</v>
       </c>
-      <c r="N16" s="132">
+      <c r="N16" s="133">
         <f t="shared" si="0"/>
         <v>3795.96346493813</v>
       </c>
-      <c r="O16" s="125"/>
-      <c r="P16" s="125"/>
-      <c r="Q16" s="125"/>
+      <c r="O16" s="126"/>
+      <c r="P16" s="126"/>
+      <c r="Q16" s="126"/>
     </row>
     <row r="17" spans="2:17">
       <c r="B17">
@@ -13669,7 +13708,7 @@
       <c r="H17" s="39">
         <v>91595</v>
       </c>
-      <c r="I17" s="125"/>
+      <c r="I17" s="126"/>
       <c r="J17" s="58"/>
       <c r="K17" s="53" t="s">
         <v>33</v>
@@ -13677,16 +13716,16 @@
       <c r="L17" s="38">
         <v>172796</v>
       </c>
-      <c r="M17" s="133">
+      <c r="M17" s="134">
         <v>39.67</v>
       </c>
-      <c r="N17" s="134">
+      <c r="N17" s="135">
         <f t="shared" si="0"/>
         <v>4355.83564406352</v>
       </c>
-      <c r="O17" s="125"/>
-      <c r="P17" s="125"/>
-      <c r="Q17" s="125"/>
+      <c r="O17" s="126"/>
+      <c r="P17" s="126"/>
+      <c r="Q17" s="126"/>
     </row>
     <row r="18" spans="2:17">
       <c r="B18">
@@ -13710,7 +13749,7 @@
       <c r="H18" s="39">
         <v>220593</v>
       </c>
-      <c r="I18" s="125"/>
+      <c r="I18" s="126"/>
       <c r="J18" s="54"/>
       <c r="K18" s="53" t="s">
         <v>39</v>
@@ -13718,16 +13757,16 @@
       <c r="L18" s="38">
         <v>436040</v>
       </c>
-      <c r="M18" s="131">
+      <c r="M18" s="132">
         <v>69.57</v>
       </c>
-      <c r="N18" s="132">
+      <c r="N18" s="133">
         <f t="shared" si="0"/>
         <v>6267.64409946816</v>
       </c>
-      <c r="O18" s="125"/>
-      <c r="P18" s="125"/>
-      <c r="Q18" s="125"/>
+      <c r="O18" s="126"/>
+      <c r="P18" s="126"/>
+      <c r="Q18" s="126"/>
     </row>
     <row r="19" spans="2:17">
       <c r="B19">
@@ -13751,7 +13790,7 @@
       <c r="H19" s="39">
         <v>97358</v>
       </c>
-      <c r="I19" s="125"/>
+      <c r="I19" s="126"/>
       <c r="J19" s="54"/>
       <c r="K19" s="53" t="s">
         <v>55</v>
@@ -13759,16 +13798,16 @@
       <c r="L19" s="38">
         <v>189359</v>
       </c>
-      <c r="M19" s="131">
+      <c r="M19" s="132">
         <v>113.81</v>
       </c>
-      <c r="N19" s="132">
+      <c r="N19" s="133">
         <f t="shared" si="0"/>
         <v>1663.81688779545</v>
       </c>
-      <c r="O19" s="125"/>
-      <c r="P19" s="125"/>
-      <c r="Q19" s="125"/>
+      <c r="O19" s="126"/>
+      <c r="P19" s="126"/>
+      <c r="Q19" s="126"/>
     </row>
     <row r="20" spans="2:17">
       <c r="B20">
@@ -13792,7 +13831,7 @@
       <c r="H20" s="39">
         <v>124465</v>
       </c>
-      <c r="I20" s="125"/>
+      <c r="I20" s="126"/>
       <c r="J20" s="54"/>
       <c r="K20" s="53" t="s">
         <v>39</v>
@@ -13800,16 +13839,16 @@
       <c r="L20" s="38">
         <v>242230</v>
       </c>
-      <c r="M20" s="131">
+      <c r="M20" s="132">
         <v>35.76</v>
       </c>
-      <c r="N20" s="132">
+      <c r="N20" s="133">
         <f t="shared" si="0"/>
         <v>6773.76957494407</v>
       </c>
-      <c r="O20" s="125"/>
-      <c r="P20" s="125"/>
-      <c r="Q20" s="125"/>
+      <c r="O20" s="126"/>
+      <c r="P20" s="126"/>
+      <c r="Q20" s="126"/>
     </row>
     <row r="21" spans="2:17">
       <c r="B21">
@@ -13833,7 +13872,7 @@
       <c r="H21" s="39">
         <v>30386</v>
       </c>
-      <c r="I21" s="125"/>
+      <c r="I21" s="126"/>
       <c r="J21" s="54"/>
       <c r="K21" s="53" t="s">
         <v>33</v>
@@ -13841,16 +13880,16 @@
       <c r="L21" s="38">
         <v>56980</v>
       </c>
-      <c r="M21" s="131">
+      <c r="M21" s="132">
         <v>17.28</v>
       </c>
-      <c r="N21" s="132">
+      <c r="N21" s="133">
         <f t="shared" si="0"/>
         <v>3297.4537037037</v>
       </c>
-      <c r="O21" s="125"/>
-      <c r="P21" s="125"/>
-      <c r="Q21" s="125"/>
+      <c r="O21" s="126"/>
+      <c r="P21" s="126"/>
+      <c r="Q21" s="126"/>
     </row>
     <row r="22" spans="2:17">
       <c r="B22">
@@ -13874,7 +13913,7 @@
       <c r="H22" s="39">
         <v>21840</v>
       </c>
-      <c r="I22" s="125"/>
+      <c r="I22" s="126"/>
       <c r="J22" s="54"/>
       <c r="K22" s="53" t="s">
         <v>33</v>
@@ -13882,16 +13921,16 @@
       <c r="L22" s="38">
         <v>41968</v>
       </c>
-      <c r="M22" s="131">
+      <c r="M22" s="132">
         <v>32.05</v>
       </c>
-      <c r="N22" s="132">
+      <c r="N22" s="133">
         <f t="shared" si="0"/>
         <v>1309.45397815913</v>
       </c>
-      <c r="O22" s="125"/>
-      <c r="P22" s="125"/>
-      <c r="Q22" s="125"/>
+      <c r="O22" s="126"/>
+      <c r="P22" s="126"/>
+      <c r="Q22" s="126"/>
     </row>
     <row r="23" spans="2:17">
       <c r="B23">
@@ -13915,7 +13954,7 @@
       <c r="H23" s="39">
         <v>80269</v>
       </c>
-      <c r="I23" s="125"/>
+      <c r="I23" s="126"/>
       <c r="J23" s="54"/>
       <c r="K23" s="53" t="s">
         <v>39</v>
@@ -13923,16 +13962,16 @@
       <c r="L23" s="38">
         <v>164620</v>
       </c>
-      <c r="M23" s="131">
+      <c r="M23" s="132">
         <v>103.76</v>
       </c>
-      <c r="N23" s="132">
+      <c r="N23" s="133">
         <f t="shared" si="0"/>
         <v>1586.54587509638</v>
       </c>
-      <c r="O23" s="125"/>
-      <c r="P23" s="125"/>
-      <c r="Q23" s="125"/>
+      <c r="O23" s="126"/>
+      <c r="P23" s="126"/>
+      <c r="Q23" s="126"/>
     </row>
     <row r="24" spans="2:17">
       <c r="B24">
@@ -13956,7 +13995,7 @@
       <c r="H24" s="39">
         <v>108258</v>
       </c>
-      <c r="I24" s="125"/>
+      <c r="I24" s="126"/>
       <c r="J24" s="54"/>
       <c r="K24" s="53" t="s">
         <v>27</v>
@@ -13964,16 +14003,16 @@
       <c r="L24" s="38">
         <v>224326</v>
       </c>
-      <c r="M24" s="131">
+      <c r="M24" s="132">
         <v>93.84</v>
       </c>
-      <c r="N24" s="132">
+      <c r="N24" s="133">
         <f t="shared" si="0"/>
         <v>2390.515771526</v>
       </c>
-      <c r="O24" s="125"/>
-      <c r="P24" s="125"/>
-      <c r="Q24" s="125"/>
+      <c r="O24" s="126"/>
+      <c r="P24" s="126"/>
+      <c r="Q24" s="126"/>
     </row>
     <row r="25" spans="2:17">
       <c r="B25">
@@ -13997,7 +14036,7 @@
       <c r="H25" s="39">
         <v>119632</v>
       </c>
-      <c r="I25" s="125"/>
+      <c r="I25" s="126"/>
       <c r="J25" s="54"/>
       <c r="K25" s="53" t="s">
         <v>27</v>
@@ -14005,16 +14044,16 @@
       <c r="L25" s="38">
         <v>239068</v>
       </c>
-      <c r="M25" s="131">
+      <c r="M25" s="132">
         <v>27.09</v>
       </c>
-      <c r="N25" s="132">
+      <c r="N25" s="133">
         <f t="shared" si="0"/>
         <v>8824.953857512</v>
       </c>
-      <c r="O25" s="125"/>
-      <c r="P25" s="125"/>
-      <c r="Q25" s="125"/>
+      <c r="O25" s="126"/>
+      <c r="P25" s="126"/>
+      <c r="Q25" s="126"/>
     </row>
     <row r="26" spans="2:17">
       <c r="B26">
@@ -14038,7 +14077,7 @@
       <c r="H26" s="39">
         <v>50323</v>
       </c>
-      <c r="I26" s="125"/>
+      <c r="I26" s="126"/>
       <c r="J26" s="54"/>
       <c r="K26" s="53" t="s">
         <v>39</v>
@@ -14046,16 +14085,16 @@
       <c r="L26" s="38">
         <v>102171</v>
       </c>
-      <c r="M26" s="131">
+      <c r="M26" s="132">
         <v>55.56</v>
       </c>
-      <c r="N26" s="132">
+      <c r="N26" s="133">
         <f t="shared" si="0"/>
         <v>1838.93088552916</v>
       </c>
-      <c r="O26" s="125"/>
-      <c r="P26" s="125"/>
-      <c r="Q26" s="125"/>
+      <c r="O26" s="126"/>
+      <c r="P26" s="126"/>
+      <c r="Q26" s="126"/>
     </row>
     <row r="27" spans="2:17">
       <c r="B27">
@@ -14079,7 +14118,7 @@
       <c r="H27" s="39">
         <v>67257</v>
       </c>
-      <c r="I27" s="125"/>
+      <c r="I27" s="126"/>
       <c r="J27" s="54"/>
       <c r="K27" s="53" t="s">
         <v>27</v>
@@ -14087,16 +14126,16 @@
       <c r="L27" s="38">
         <v>135384</v>
       </c>
-      <c r="M27" s="131">
+      <c r="M27" s="132">
         <v>26.59</v>
       </c>
-      <c r="N27" s="132">
+      <c r="N27" s="133">
         <f t="shared" si="0"/>
         <v>5091.5381722452</v>
       </c>
-      <c r="O27" s="125"/>
-      <c r="P27" s="125"/>
-      <c r="Q27" s="125"/>
+      <c r="O27" s="126"/>
+      <c r="P27" s="126"/>
+      <c r="Q27" s="126"/>
     </row>
     <row r="28" spans="2:17">
       <c r="B28">
@@ -14120,7 +14159,7 @@
       <c r="H28" s="39">
         <v>65608</v>
       </c>
-      <c r="I28" s="125"/>
+      <c r="I28" s="126"/>
       <c r="J28" s="54"/>
       <c r="K28" s="53" t="s">
         <v>27</v>
@@ -14128,16 +14167,16 @@
       <c r="L28" s="38">
         <v>130772</v>
       </c>
-      <c r="M28" s="131">
+      <c r="M28" s="132">
         <v>17.57</v>
       </c>
-      <c r="N28" s="132">
+      <c r="N28" s="133">
         <f t="shared" si="0"/>
         <v>7442.9140580535</v>
       </c>
-      <c r="O28" s="125"/>
-      <c r="P28" s="125"/>
-      <c r="Q28" s="125"/>
+      <c r="O28" s="126"/>
+      <c r="P28" s="126"/>
+      <c r="Q28" s="126"/>
     </row>
     <row r="29" spans="2:17">
       <c r="B29">
@@ -14161,7 +14200,7 @@
       <c r="H29" s="39">
         <v>21044</v>
       </c>
-      <c r="I29" s="125"/>
+      <c r="I29" s="126"/>
       <c r="J29" s="54"/>
       <c r="K29" s="53" t="s">
         <v>55</v>
@@ -14169,16 +14208,16 @@
       <c r="L29" s="38">
         <v>41395</v>
       </c>
-      <c r="M29" s="131">
+      <c r="M29" s="132">
         <v>77.12</v>
       </c>
-      <c r="N29" s="132">
+      <c r="N29" s="133">
         <f t="shared" si="0"/>
         <v>536.760892116183</v>
       </c>
-      <c r="O29" s="125"/>
-      <c r="P29" s="125"/>
-      <c r="Q29" s="125"/>
+      <c r="O29" s="126"/>
+      <c r="P29" s="126"/>
+      <c r="Q29" s="126"/>
     </row>
     <row r="30" spans="2:17">
       <c r="B30">
@@ -14202,7 +14241,7 @@
       <c r="H30" s="39">
         <v>41273</v>
       </c>
-      <c r="I30" s="125"/>
+      <c r="I30" s="126"/>
       <c r="J30" s="54"/>
       <c r="K30" s="53" t="s">
         <v>27</v>
@@ -14210,16 +14249,16 @@
       <c r="L30" s="38">
         <v>84428</v>
       </c>
-      <c r="M30" s="131">
+      <c r="M30" s="132">
         <v>22.14</v>
       </c>
-      <c r="N30" s="132">
+      <c r="N30" s="133">
         <f t="shared" si="0"/>
         <v>3813.369467028</v>
       </c>
-      <c r="O30" s="125"/>
-      <c r="P30" s="125"/>
-      <c r="Q30" s="125"/>
+      <c r="O30" s="126"/>
+      <c r="P30" s="126"/>
+      <c r="Q30" s="126"/>
     </row>
     <row r="31" spans="2:17">
       <c r="B31">
@@ -14243,7 +14282,7 @@
       <c r="H31" s="39">
         <v>16651</v>
       </c>
-      <c r="I31" s="125"/>
+      <c r="I31" s="126"/>
       <c r="J31" s="54"/>
       <c r="K31" s="53" t="s">
         <v>33</v>
@@ -14251,16 +14290,16 @@
       <c r="L31" s="38">
         <v>31552</v>
       </c>
-      <c r="M31" s="131">
+      <c r="M31" s="132">
         <v>17.04</v>
       </c>
-      <c r="N31" s="132">
+      <c r="N31" s="133">
         <f t="shared" si="0"/>
         <v>1851.64319248826</v>
       </c>
-      <c r="O31" s="125"/>
-      <c r="P31" s="125"/>
-      <c r="Q31" s="125"/>
+      <c r="O31" s="126"/>
+      <c r="P31" s="126"/>
+      <c r="Q31" s="126"/>
     </row>
     <row r="32" spans="2:17">
       <c r="B32">
@@ -14284,7 +14323,7 @@
       <c r="H32" s="39">
         <v>23875</v>
       </c>
-      <c r="I32" s="125"/>
+      <c r="I32" s="126"/>
       <c r="J32" s="54"/>
       <c r="K32" s="53" t="s">
         <v>39</v>
@@ -14292,16 +14331,16 @@
       <c r="L32" s="38">
         <v>48486</v>
       </c>
-      <c r="M32" s="131">
+      <c r="M32" s="132">
         <v>13.34</v>
       </c>
-      <c r="N32" s="132">
+      <c r="N32" s="133">
         <f t="shared" si="0"/>
         <v>3634.63268365817</v>
       </c>
-      <c r="O32" s="125"/>
-      <c r="P32" s="125"/>
-      <c r="Q32" s="125"/>
+      <c r="O32" s="126"/>
+      <c r="P32" s="126"/>
+      <c r="Q32" s="126"/>
     </row>
     <row r="33" spans="2:17">
       <c r="B33">
@@ -14325,7 +14364,7 @@
       <c r="H33" s="39">
         <v>15938</v>
       </c>
-      <c r="I33" s="125"/>
+      <c r="I33" s="126"/>
       <c r="J33" s="54"/>
       <c r="K33" s="53" t="s">
         <v>39</v>
@@ -14333,16 +14372,16 @@
       <c r="L33" s="38">
         <v>31161</v>
       </c>
-      <c r="M33" s="131">
+      <c r="M33" s="132">
         <v>17.23</v>
       </c>
-      <c r="N33" s="132">
+      <c r="N33" s="133">
         <f t="shared" si="0"/>
         <v>1808.53163087638</v>
       </c>
-      <c r="O33" s="125"/>
-      <c r="P33" s="125"/>
-      <c r="Q33" s="125"/>
+      <c r="O33" s="126"/>
+      <c r="P33" s="126"/>
+      <c r="Q33" s="126"/>
     </row>
     <row r="34" spans="2:17">
       <c r="B34">
@@ -14366,7 +14405,7 @@
       <c r="H34" s="39">
         <v>14265</v>
       </c>
-      <c r="I34" s="125"/>
+      <c r="I34" s="126"/>
       <c r="J34" s="54"/>
       <c r="K34" s="53" t="s">
         <v>39</v>
@@ -14374,16 +14413,16 @@
       <c r="L34" s="38">
         <v>27583</v>
       </c>
-      <c r="M34" s="131">
+      <c r="M34" s="132">
         <v>9.08</v>
       </c>
-      <c r="N34" s="132">
+      <c r="N34" s="133">
         <f t="shared" si="0"/>
         <v>3037.77533039648</v>
       </c>
-      <c r="O34" s="125"/>
-      <c r="P34" s="125"/>
-      <c r="Q34" s="125"/>
+      <c r="O34" s="126"/>
+      <c r="P34" s="126"/>
+      <c r="Q34" s="126"/>
     </row>
     <row r="35" spans="2:17">
       <c r="B35">
@@ -14407,7 +14446,7 @@
       <c r="H35" s="39">
         <v>4628</v>
       </c>
-      <c r="I35" s="125"/>
+      <c r="I35" s="126"/>
       <c r="J35" s="54"/>
       <c r="K35" s="53" t="s">
         <v>55</v>
@@ -14415,16 +14454,16 @@
       <c r="L35" s="38">
         <v>9309</v>
       </c>
-      <c r="M35" s="131">
+      <c r="M35" s="132">
         <v>19.99</v>
       </c>
-      <c r="N35" s="132">
+      <c r="N35" s="133">
         <f t="shared" si="0"/>
         <v>465.68284142071</v>
       </c>
-      <c r="O35" s="125"/>
-      <c r="P35" s="125"/>
-      <c r="Q35" s="125"/>
+      <c r="O35" s="126"/>
+      <c r="P35" s="126"/>
+      <c r="Q35" s="126"/>
     </row>
     <row r="36" spans="2:17">
       <c r="B36">
@@ -14448,7 +14487,7 @@
       <c r="H36" s="39">
         <v>8606</v>
       </c>
-      <c r="I36" s="125"/>
+      <c r="I36" s="126"/>
       <c r="J36" s="54"/>
       <c r="K36" s="53" t="s">
         <v>55</v>
@@ -14456,16 +14495,16 @@
       <c r="L36" s="38">
         <v>17058</v>
       </c>
-      <c r="M36" s="131">
+      <c r="M36" s="132">
         <v>14.38</v>
       </c>
-      <c r="N36" s="132">
+      <c r="N36" s="133">
         <f t="shared" si="0"/>
         <v>1186.23087621697</v>
       </c>
-      <c r="O36" s="125"/>
-      <c r="P36" s="125"/>
-      <c r="Q36" s="125"/>
+      <c r="O36" s="126"/>
+      <c r="P36" s="126"/>
+      <c r="Q36" s="126"/>
     </row>
     <row r="37" spans="2:17">
       <c r="B37">
@@ -14489,7 +14528,7 @@
       <c r="H37" s="39">
         <v>5409</v>
       </c>
-      <c r="I37" s="125"/>
+      <c r="I37" s="126"/>
       <c r="J37" s="54"/>
       <c r="K37" s="53" t="s">
         <v>55</v>
@@ -14497,16 +14536,16 @@
       <c r="L37" s="38">
         <v>10710</v>
       </c>
-      <c r="M37" s="131">
+      <c r="M37" s="132">
         <v>37.75</v>
       </c>
-      <c r="N37" s="132">
+      <c r="N37" s="133">
         <f t="shared" si="0"/>
         <v>283.708609271523</v>
       </c>
-      <c r="O37" s="125"/>
-      <c r="P37" s="125"/>
-      <c r="Q37" s="125"/>
+      <c r="O37" s="126"/>
+      <c r="P37" s="126"/>
+      <c r="Q37" s="126"/>
     </row>
     <row r="38" spans="2:17">
       <c r="B38">
@@ -14530,7 +14569,7 @@
       <c r="H38" s="39">
         <v>4872</v>
       </c>
-      <c r="I38" s="125"/>
+      <c r="I38" s="126"/>
       <c r="J38" s="54"/>
       <c r="K38" s="53" t="s">
         <v>55</v>
@@ -14538,16 +14577,16 @@
       <c r="L38" s="38">
         <v>9576</v>
       </c>
-      <c r="M38" s="131">
+      <c r="M38" s="132">
         <v>224.61</v>
       </c>
-      <c r="N38" s="132">
+      <c r="N38" s="133">
         <f t="shared" si="0"/>
         <v>42.6338987578469</v>
       </c>
-      <c r="O38" s="125"/>
-      <c r="P38" s="125"/>
-      <c r="Q38" s="125"/>
+      <c r="O38" s="126"/>
+      <c r="P38" s="126"/>
+      <c r="Q38" s="126"/>
     </row>
     <row r="39" spans="2:17">
       <c r="B39">
@@ -14571,7 +14610,7 @@
       <c r="H39" s="39">
         <v>9342</v>
       </c>
-      <c r="I39" s="125"/>
+      <c r="I39" s="126"/>
       <c r="J39" s="54"/>
       <c r="K39" s="53" t="s">
         <v>55</v>
@@ -14579,16 +14618,16 @@
       <c r="L39" s="38">
         <v>18155</v>
       </c>
-      <c r="M39" s="131">
+      <c r="M39" s="132">
         <v>6.55</v>
       </c>
-      <c r="N39" s="132">
+      <c r="N39" s="133">
         <f t="shared" si="0"/>
         <v>2771.75572519084</v>
       </c>
-      <c r="O39" s="125"/>
-      <c r="P39" s="125"/>
-      <c r="Q39" s="125"/>
+      <c r="O39" s="126"/>
+      <c r="P39" s="126"/>
+      <c r="Q39" s="126"/>
     </row>
     <row r="40" spans="2:17">
       <c r="B40">
@@ -14612,7 +14651,7 @@
       <c r="H40" s="39">
         <v>5799</v>
       </c>
-      <c r="I40" s="125"/>
+      <c r="I40" s="126"/>
       <c r="J40" s="54"/>
       <c r="K40" s="53" t="s">
         <v>55</v>
@@ -14620,16 +14659,16 @@
       <c r="L40" s="38">
         <v>11015</v>
       </c>
-      <c r="M40" s="131">
+      <c r="M40" s="132">
         <v>92.86</v>
       </c>
-      <c r="N40" s="132">
+      <c r="N40" s="133">
         <f t="shared" si="0"/>
         <v>118.619427094551</v>
       </c>
-      <c r="O40" s="125"/>
-      <c r="P40" s="125"/>
-      <c r="Q40" s="125"/>
+      <c r="O40" s="126"/>
+      <c r="P40" s="126"/>
+      <c r="Q40" s="126"/>
     </row>
     <row r="41" spans="2:17">
       <c r="B41">
@@ -14653,7 +14692,7 @@
       <c r="H41" s="39">
         <v>3590</v>
       </c>
-      <c r="I41" s="125"/>
+      <c r="I41" s="126"/>
       <c r="J41" s="54"/>
       <c r="K41" s="53" t="s">
         <v>55</v>
@@ -14661,16 +14700,16 @@
       <c r="L41" s="38">
         <v>6746</v>
       </c>
-      <c r="M41" s="131">
+      <c r="M41" s="132">
         <v>7.05</v>
       </c>
-      <c r="N41" s="132">
+      <c r="N41" s="133">
         <f t="shared" si="0"/>
         <v>956.879432624114</v>
       </c>
-      <c r="O41" s="125"/>
-      <c r="P41" s="125"/>
-      <c r="Q41" s="125"/>
+      <c r="O41" s="126"/>
+      <c r="P41" s="126"/>
+      <c r="Q41" s="126"/>
     </row>
     <row r="42" spans="2:17">
       <c r="B42">
@@ -14694,7 +14733,7 @@
       <c r="H42" s="39">
         <v>12609</v>
       </c>
-      <c r="I42" s="125"/>
+      <c r="I42" s="126"/>
       <c r="J42" s="54"/>
       <c r="K42" s="53" t="s">
         <v>55</v>
@@ -14702,16 +14741,16 @@
       <c r="L42" s="38">
         <v>23585</v>
       </c>
-      <c r="M42" s="131">
+      <c r="M42" s="132">
         <v>40.97</v>
       </c>
-      <c r="N42" s="132">
+      <c r="N42" s="133">
         <f t="shared" si="0"/>
         <v>575.665120820112</v>
       </c>
-      <c r="O42" s="125"/>
-      <c r="P42" s="125"/>
-      <c r="Q42" s="125"/>
+      <c r="O42" s="126"/>
+      <c r="P42" s="126"/>
+      <c r="Q42" s="126"/>
     </row>
     <row r="43" spans="2:17">
       <c r="B43">
@@ -14735,7 +14774,7 @@
       <c r="H43" s="39">
         <v>18805</v>
       </c>
-      <c r="I43" s="125"/>
+      <c r="I43" s="126"/>
       <c r="J43" s="81"/>
       <c r="K43" s="53" t="s">
         <v>27</v>
@@ -14743,16 +14782,16 @@
       <c r="L43" s="38">
         <v>39319</v>
       </c>
-      <c r="M43" s="135">
+      <c r="M43" s="136">
         <v>34.28</v>
       </c>
-      <c r="N43" s="136">
+      <c r="N43" s="137">
         <f t="shared" si="0"/>
         <v>1146.99533255543</v>
       </c>
-      <c r="O43" s="125"/>
-      <c r="P43" s="125"/>
-      <c r="Q43" s="125"/>
+      <c r="O43" s="126"/>
+      <c r="P43" s="126"/>
+      <c r="Q43" s="126"/>
     </row>
     <row r="44" ht="17.25" spans="2:17">
       <c r="B44">
@@ -14776,7 +14815,7 @@
       <c r="H44" s="39">
         <v>1498</v>
       </c>
-      <c r="I44" s="125"/>
+      <c r="I44" s="126"/>
       <c r="J44" s="83"/>
       <c r="K44" s="82" t="s">
         <v>27</v>
@@ -14784,16 +14823,16 @@
       <c r="L44" s="38">
         <v>3061</v>
       </c>
-      <c r="M44" s="137">
+      <c r="M44" s="138">
         <v>71.24</v>
       </c>
-      <c r="N44" s="138">
+      <c r="N44" s="139">
         <f t="shared" si="0"/>
         <v>42.9674340258282</v>
       </c>
-      <c r="O44" s="125"/>
-      <c r="P44" s="125"/>
-      <c r="Q44" s="125"/>
+      <c r="O44" s="126"/>
+      <c r="P44" s="126"/>
+      <c r="Q44" s="126"/>
     </row>
     <row r="49" ht="27.75" spans="3:17">
       <c r="C49" s="104" t="s">
@@ -14821,27 +14860,27 @@
       <c r="D50" s="107" t="s">
         <v>212</v>
       </c>
-      <c r="E50" s="117"/>
-      <c r="F50" s="117"/>
-      <c r="G50" s="117"/>
-      <c r="H50" s="117"/>
-      <c r="I50" s="117"/>
-      <c r="J50" s="117"/>
+      <c r="E50" s="118"/>
+      <c r="F50" s="118"/>
+      <c r="G50" s="118"/>
+      <c r="H50" s="118"/>
+      <c r="I50" s="118"/>
+      <c r="J50" s="118"/>
       <c r="K50" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="L50" s="117" t="s">
+      <c r="L50" s="118" t="s">
         <v>213</v>
       </c>
-      <c r="M50" s="121" t="s">
+      <c r="M50" s="122" t="s">
         <v>188</v>
       </c>
-      <c r="N50" s="121" t="s">
+      <c r="N50" s="122" t="s">
         <v>189</v>
       </c>
-      <c r="O50" s="117"/>
-      <c r="P50" s="117"/>
-      <c r="Q50" s="117"/>
+      <c r="O50" s="118"/>
+      <c r="P50" s="118"/>
+      <c r="Q50" s="118"/>
     </row>
     <row r="51" ht="17.25" customHeight="1" spans="3:17">
       <c r="C51" s="108" t="s">
@@ -14850,30 +14889,30 @@
       <c r="D51" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="E51" s="118"/>
-      <c r="F51" s="118"/>
-      <c r="G51" s="118"/>
-      <c r="H51" s="118"/>
-      <c r="I51" s="118"/>
-      <c r="J51" s="118"/>
+      <c r="E51" s="119"/>
+      <c r="F51" s="119"/>
+      <c r="G51" s="119"/>
+      <c r="H51" s="119"/>
+      <c r="I51" s="119"/>
+      <c r="J51" s="119"/>
       <c r="K51" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="L51" s="139">
+      <c r="L51" s="140">
         <f t="shared" ref="L51:L56" si="1">SUMIFS($L$12:$L$44,$K$12:$K$44,K51)</f>
         <v>3760467</v>
       </c>
-      <c r="M51" s="140">
+      <c r="M51" s="141">
         <f t="shared" ref="M51:M56" si="2">SUMIFS($M$12:$M$44,$K$12:$K$44,K51)</f>
         <v>437.56</v>
       </c>
-      <c r="N51" s="132">
+      <c r="N51" s="133">
         <f t="shared" ref="N51:N56" si="3">L51/M51</f>
         <v>8594.17451320962</v>
       </c>
-      <c r="O51" s="140"/>
-      <c r="P51" s="140"/>
-      <c r="Q51" s="140"/>
+      <c r="O51" s="141"/>
+      <c r="P51" s="141"/>
+      <c r="Q51" s="141"/>
     </row>
     <row r="52" ht="17.25" customHeight="1" spans="3:17">
       <c r="C52" s="108" t="s">
@@ -14882,30 +14921,30 @@
       <c r="D52" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="E52" s="118"/>
-      <c r="F52" s="118"/>
-      <c r="G52" s="118"/>
-      <c r="H52" s="118"/>
-      <c r="I52" s="118"/>
-      <c r="J52" s="118"/>
+      <c r="E52" s="119"/>
+      <c r="F52" s="119"/>
+      <c r="G52" s="119"/>
+      <c r="H52" s="119"/>
+      <c r="I52" s="119"/>
+      <c r="J52" s="119"/>
       <c r="K52" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="L52" s="139">
+      <c r="L52" s="140">
         <f t="shared" si="1"/>
         <v>1539284</v>
       </c>
-      <c r="M52" s="140">
+      <c r="M52" s="141">
         <f t="shared" si="2"/>
         <v>143.01</v>
       </c>
-      <c r="N52" s="132">
+      <c r="N52" s="133">
         <f t="shared" si="3"/>
         <v>10763.471085938</v>
       </c>
-      <c r="O52" s="140"/>
-      <c r="P52" s="140"/>
-      <c r="Q52" s="140"/>
+      <c r="O52" s="141"/>
+      <c r="P52" s="141"/>
+      <c r="Q52" s="141"/>
     </row>
     <row r="53" ht="17.25" customHeight="1" spans="3:17">
       <c r="C53" s="108" t="s">
@@ -14914,30 +14953,30 @@
       <c r="D53" s="109" t="s">
         <v>214</v>
       </c>
-      <c r="E53" s="118"/>
-      <c r="F53" s="118"/>
-      <c r="G53" s="118"/>
-      <c r="H53" s="118"/>
-      <c r="I53" s="118"/>
-      <c r="J53" s="118"/>
+      <c r="E53" s="119"/>
+      <c r="F53" s="119"/>
+      <c r="G53" s="119"/>
+      <c r="H53" s="119"/>
+      <c r="I53" s="119"/>
+      <c r="J53" s="119"/>
       <c r="K53" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="L53" s="139">
+      <c r="L53" s="140">
         <f t="shared" si="1"/>
         <v>696443</v>
       </c>
-      <c r="M53" s="140">
+      <c r="M53" s="141">
         <f t="shared" si="2"/>
         <v>206.86</v>
       </c>
-      <c r="N53" s="132">
+      <c r="N53" s="133">
         <f t="shared" si="3"/>
         <v>3366.73595668568</v>
       </c>
-      <c r="O53" s="140"/>
-      <c r="P53" s="140"/>
-      <c r="Q53" s="140"/>
+      <c r="O53" s="141"/>
+      <c r="P53" s="141"/>
+      <c r="Q53" s="141"/>
     </row>
     <row r="54" ht="17.25" customHeight="1" spans="3:17">
       <c r="C54" s="108" t="s">
@@ -14946,30 +14985,30 @@
       <c r="D54" s="109" t="s">
         <v>215</v>
       </c>
-      <c r="E54" s="118"/>
-      <c r="F54" s="118"/>
-      <c r="G54" s="118"/>
-      <c r="H54" s="118"/>
-      <c r="I54" s="118"/>
-      <c r="J54" s="118"/>
+      <c r="E54" s="119"/>
+      <c r="F54" s="119"/>
+      <c r="G54" s="119"/>
+      <c r="H54" s="119"/>
+      <c r="I54" s="119"/>
+      <c r="J54" s="119"/>
       <c r="K54" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="L54" s="139">
+      <c r="L54" s="140">
         <f t="shared" si="1"/>
         <v>1579555</v>
       </c>
-      <c r="M54" s="140">
+      <c r="M54" s="141">
         <f t="shared" si="2"/>
         <v>621.66</v>
       </c>
-      <c r="N54" s="132">
+      <c r="N54" s="133">
         <f t="shared" si="3"/>
         <v>2540.8663899881</v>
       </c>
-      <c r="O54" s="140"/>
-      <c r="P54" s="140"/>
-      <c r="Q54" s="140"/>
+      <c r="O54" s="141"/>
+      <c r="P54" s="141"/>
+      <c r="Q54" s="141"/>
     </row>
     <row r="55" ht="17.25" customHeight="1" spans="3:17">
       <c r="C55" s="108" t="s">
@@ -14978,30 +15017,30 @@
       <c r="D55" s="109" t="s">
         <v>216</v>
       </c>
-      <c r="E55" s="118"/>
-      <c r="F55" s="118"/>
-      <c r="G55" s="118"/>
-      <c r="H55" s="118"/>
-      <c r="I55" s="118"/>
-      <c r="J55" s="118"/>
+      <c r="E55" s="119"/>
+      <c r="F55" s="119"/>
+      <c r="G55" s="119"/>
+      <c r="H55" s="119"/>
+      <c r="I55" s="119"/>
+      <c r="J55" s="119"/>
       <c r="K55" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="L55" s="139">
+      <c r="L55" s="140">
         <f t="shared" si="1"/>
         <v>1309961</v>
       </c>
-      <c r="M55" s="140">
+      <c r="M55" s="141">
         <f t="shared" si="2"/>
         <v>372.18</v>
       </c>
-      <c r="N55" s="132">
+      <c r="N55" s="133">
         <f t="shared" si="3"/>
         <v>3519.69745821914</v>
       </c>
-      <c r="O55" s="140"/>
-      <c r="P55" s="140"/>
-      <c r="Q55" s="140"/>
+      <c r="O55" s="141"/>
+      <c r="P55" s="141"/>
+      <c r="Q55" s="141"/>
     </row>
     <row r="56" ht="17.25" customHeight="1" spans="3:17">
       <c r="C56" s="111" t="s">
@@ -15010,30 +15049,30 @@
       <c r="D56" s="109" t="s">
         <v>217</v>
       </c>
-      <c r="E56" s="118"/>
-      <c r="F56" s="118"/>
-      <c r="G56" s="118"/>
-      <c r="H56" s="118"/>
-      <c r="I56" s="118"/>
-      <c r="J56" s="118"/>
+      <c r="E56" s="119"/>
+      <c r="F56" s="119"/>
+      <c r="G56" s="119"/>
+      <c r="H56" s="119"/>
+      <c r="I56" s="119"/>
+      <c r="J56" s="119"/>
       <c r="K56" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="L56" s="139">
+      <c r="L56" s="140">
         <f t="shared" si="1"/>
         <v>336908</v>
       </c>
-      <c r="M56" s="140">
+      <c r="M56" s="141">
         <f t="shared" si="2"/>
         <v>635.09</v>
       </c>
-      <c r="N56" s="132">
+      <c r="N56" s="133">
         <f t="shared" si="3"/>
         <v>530.488592168039</v>
       </c>
-      <c r="O56" s="140"/>
-      <c r="P56" s="140"/>
-      <c r="Q56" s="140"/>
+      <c r="O56" s="141"/>
+      <c r="P56" s="141"/>
+      <c r="Q56" s="141"/>
     </row>
     <row r="57" ht="17.25"/>
   </sheetData>
@@ -15061,169 +15100,314 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5714285714286" defaultRowHeight="16.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11.5714285714286" defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="2:4">
-      <c r="B1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
         <v>218</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="2:13">
+      <c r="B2" s="114" t="s">
         <v>219</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" s="114" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="D2" s="114" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="114" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="114" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="114" t="s">
+        <v>224</v>
+      </c>
+      <c r="H2" s="114" t="s">
+        <v>225</v>
+      </c>
+      <c r="I2" s="114" t="s">
+        <v>226</v>
+      </c>
+      <c r="J2" s="114" t="s">
+        <v>227</v>
+      </c>
+      <c r="K2" s="114" t="s">
+        <v>228</v>
+      </c>
+      <c r="L2" s="114" t="s">
+        <v>229</v>
+      </c>
+      <c r="M2" s="114" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3">
         <v>9163279</v>
       </c>
-      <c r="C2">
+      <c r="C3">
+        <v>9160412</v>
+      </c>
+      <c r="D3">
+        <v>9157211</v>
+      </c>
+      <c r="E3">
+        <v>9161113</v>
+      </c>
+      <c r="F3">
+        <v>9177834</v>
+      </c>
+      <c r="G3">
+        <v>9180700</v>
+      </c>
+      <c r="H3">
+        <v>9181389</v>
+      </c>
+      <c r="I3">
+        <v>9180457</v>
+      </c>
+      <c r="J3">
+        <v>9179666</v>
+      </c>
+      <c r="K3">
+        <v>9179835</v>
+      </c>
+      <c r="L3">
+        <v>9183257</v>
+      </c>
+      <c r="M3">
+        <v>9182071</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4">
         <v>9181625</v>
       </c>
-      <c r="D2">
+      <c r="C4">
+        <v>9178503</v>
+      </c>
+      <c r="D4">
+        <v>9175042</v>
+      </c>
+      <c r="E4">
+        <v>9180510</v>
+      </c>
+      <c r="F4">
+        <v>9197925</v>
+      </c>
+      <c r="G4">
+        <v>9199871</v>
+      </c>
+      <c r="H4">
+        <v>9199590</v>
+      </c>
+      <c r="I4">
+        <v>9199389</v>
+      </c>
+      <c r="J4">
+        <v>9199037</v>
+      </c>
+      <c r="K4">
+        <v>9200166</v>
+      </c>
+      <c r="L4">
+        <v>9203069</v>
+      </c>
+      <c r="M4">
+        <v>9202523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5">
         <v>9201825</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="C5">
+        <v>9198646</v>
+      </c>
+      <c r="D5">
+        <v>9196411</v>
+      </c>
+      <c r="E5">
+        <v>9204965</v>
+      </c>
+      <c r="F5">
+        <v>9222618</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="114" t="s">
+        <v>219</v>
+      </c>
+      <c r="B9">
+        <v>9163279</v>
+      </c>
+      <c r="C9">
+        <v>9181625</v>
+      </c>
+      <c r="D9">
+        <v>9201825</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="114" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10">
         <v>9160412</v>
       </c>
-      <c r="C3">
+      <c r="C10">
         <v>9178503</v>
       </c>
-      <c r="D3">
+      <c r="D10">
         <v>9198646</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
+    <row r="11" spans="1:4">
+      <c r="A11" s="114" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11">
         <v>9157211</v>
       </c>
-      <c r="C4">
+      <c r="C11">
         <v>9175042</v>
       </c>
-      <c r="D4">
+      <c r="D11">
         <v>9196411</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
+    <row r="12" spans="1:4">
+      <c r="A12" s="114" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12">
         <v>9161113</v>
       </c>
-      <c r="C5">
+      <c r="C12">
         <v>9180510</v>
       </c>
-      <c r="D5">
+      <c r="D12">
         <v>9204965</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
+    <row r="13" spans="1:4">
+      <c r="A13" s="114" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13">
         <v>9177834</v>
       </c>
-      <c r="C6">
+      <c r="C13">
         <v>9197925</v>
       </c>
-      <c r="D6">
+      <c r="D13">
         <v>9222618</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
+    <row r="14" spans="1:3">
+      <c r="A14" s="114" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14">
         <v>9180700</v>
       </c>
-      <c r="C7">
+      <c r="C14">
         <v>9199871</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
+    <row r="15" spans="1:3">
+      <c r="A15" s="114" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15">
         <v>9181389</v>
       </c>
-      <c r="C8">
+      <c r="C15">
         <v>9199590</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
+    <row r="16" spans="1:3">
+      <c r="A16" s="114" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16">
         <v>9180457</v>
       </c>
-      <c r="C9">
+      <c r="C16">
         <v>9199389</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
+    <row r="17" spans="1:3">
+      <c r="A17" s="114" t="s">
+        <v>227</v>
+      </c>
+      <c r="B17">
         <v>9179666</v>
       </c>
-      <c r="C10">
+      <c r="C17">
         <v>9199037</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
+    <row r="18" spans="1:3">
+      <c r="A18" s="114" t="s">
+        <v>228</v>
+      </c>
+      <c r="B18">
         <v>9179835</v>
       </c>
-      <c r="C11">
+      <c r="C18">
         <v>9200166</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
+    <row r="19" spans="1:3">
+      <c r="A19" s="114" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19">
         <v>9183257</v>
       </c>
-      <c r="C12">
+      <c r="C19">
         <v>9203069</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
+    <row r="20" spans="1:3">
+      <c r="A20" s="114" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20">
         <v>9182071</v>
       </c>
-      <c r="C13">
+      <c r="C20">
         <v>9202523</v>
       </c>
     </row>
@@ -15269,10 +15453,10 @@
       <c r="D3" s="94"/>
       <c r="E3" s="94"/>
       <c r="F3" s="94" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="G3" s="94" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="H3" s="94" t="s">
         <v>183</v>
@@ -16118,7 +16302,7 @@
       <c r="C49" s="104"/>
       <c r="D49" s="105"/>
       <c r="E49" s="105" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" ht="24.75" spans="3:10">
@@ -16128,19 +16312,19 @@
         <v>8</v>
       </c>
       <c r="F50" s="94" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="G50" s="94" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="H50" s="94" t="s">
         <v>183</v>
       </c>
       <c r="I50" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="J50" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" ht="19.5" spans="3:10">
@@ -16356,21 +16540,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="D1" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="B2">
         <v>2018</v>
@@ -16384,7 +16568,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="B3" s="90">
         <v>2018</v>
@@ -16398,7 +16582,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="B4" s="90">
         <v>2018</v>
@@ -16412,7 +16596,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="B5" s="90">
         <v>2018</v>
@@ -16426,7 +16610,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="B6" s="90">
         <v>2018</v>
@@ -16440,7 +16624,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="B7" s="90">
         <v>2018</v>
@@ -16454,7 +16638,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="B8" s="90">
         <v>2018</v>
@@ -16468,7 +16652,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="B9" s="90">
         <v>2018</v>
@@ -16482,7 +16666,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="B10" s="90">
         <v>2018</v>
@@ -16496,7 +16680,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="B11" s="90">
         <v>2018</v>
@@ -16510,7 +16694,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="B12" s="90">
         <v>2018</v>
@@ -16524,7 +16708,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="B13" s="90">
         <v>2018</v>
@@ -16538,7 +16722,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="B14">
         <v>2019</v>
@@ -16552,7 +16736,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="B15" s="90">
         <v>2019</v>
@@ -16566,7 +16750,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="B16" s="90">
         <v>2019</v>
@@ -16580,7 +16764,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="B17" s="90">
         <v>2019</v>
@@ -16594,7 +16778,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="B18" s="90">
         <v>2019</v>
@@ -16608,7 +16792,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="B19" s="90">
         <v>2019</v>
@@ -16622,7 +16806,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="B20" s="90">
         <v>2019</v>
@@ -16636,7 +16820,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="B21" s="90">
         <v>2019</v>
@@ -16650,7 +16834,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="B22" s="90">
         <v>2019</v>
@@ -16664,7 +16848,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="B23" s="90">
         <v>2019</v>
@@ -16678,7 +16862,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="B24" s="90">
         <v>2019</v>
@@ -16692,7 +16876,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="B25" s="90">
         <v>2019</v>
@@ -16706,7 +16890,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="B26">
         <v>2020</v>
@@ -16720,7 +16904,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="B27" s="90">
         <v>2020</v>
@@ -16734,7 +16918,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="B28" s="90">
         <v>2020</v>
@@ -16748,7 +16932,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="B29" s="90">
         <v>2020</v>
@@ -16762,7 +16946,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="B30" s="90">
         <v>2020</v>
@@ -16836,7 +17020,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="63" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" ht="18" customHeight="1" spans="1:15">
@@ -16845,26 +17029,26 @@
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="14" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>191</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="64" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
       <c r="M4" s="67" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="N4" s="68" t="s">
         <v>189</v>
@@ -16886,19 +17070,19 @@
         <v>187</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="N5" s="70" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="O5" s="69"/>
     </row>
@@ -16944,7 +17128,7 @@
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="29" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="31">
@@ -17105,7 +17289,7 @@
     <row r="12" ht="24" customHeight="1" spans="3:15">
       <c r="C12" s="34"/>
       <c r="D12" s="50" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="E12" s="36"/>
       <c r="F12" s="37">
@@ -17140,7 +17324,7 @@
     <row r="13" ht="24" customHeight="1" spans="3:15">
       <c r="C13" s="34"/>
       <c r="D13" s="51" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="37">
@@ -17175,7 +17359,7 @@
     <row r="14" ht="24" customHeight="1" spans="3:15">
       <c r="C14" s="34"/>
       <c r="D14" s="50" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="E14" s="36"/>
       <c r="F14" s="37">
@@ -17210,7 +17394,7 @@
     <row r="15" ht="24" customHeight="1" spans="3:15">
       <c r="C15" s="34"/>
       <c r="D15" s="50" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="37">
@@ -17245,7 +17429,7 @@
     <row r="16" ht="24" customHeight="1" spans="3:15">
       <c r="C16" s="34"/>
       <c r="D16" s="50" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="E16" s="36"/>
       <c r="F16" s="37">
@@ -17280,7 +17464,7 @@
     <row r="17" ht="24" customHeight="1" spans="3:15">
       <c r="C17" s="34"/>
       <c r="D17" s="50" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="E17" s="36"/>
       <c r="F17" s="37">
@@ -17315,7 +17499,7 @@
     <row r="18" ht="24" customHeight="1" spans="3:15">
       <c r="C18" s="34"/>
       <c r="D18" s="51" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="E18" s="52"/>
       <c r="F18" s="37">
@@ -17350,7 +17534,7 @@
     <row r="19" ht="24" customHeight="1" spans="3:15">
       <c r="C19" s="34"/>
       <c r="D19" s="50" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="E19" s="36"/>
       <c r="F19" s="37">
@@ -17385,7 +17569,7 @@
     <row r="20" ht="24" customHeight="1" spans="3:15">
       <c r="C20" s="34"/>
       <c r="D20" s="50" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="E20" s="36"/>
       <c r="F20" s="37">
@@ -17420,7 +17604,7 @@
     <row r="21" ht="24" customHeight="1" spans="3:15">
       <c r="C21" s="34"/>
       <c r="D21" s="50" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="E21" s="36"/>
       <c r="F21" s="37">
@@ -17455,7 +17639,7 @@
     <row r="22" ht="24" customHeight="1" spans="3:15">
       <c r="C22" s="34"/>
       <c r="D22" s="50" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="E22" s="36"/>
       <c r="F22" s="37">
@@ -17490,7 +17674,7 @@
     <row r="23" ht="24" customHeight="1" spans="3:15">
       <c r="C23" s="34"/>
       <c r="D23" s="50" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="E23" s="36"/>
       <c r="F23" s="37">
@@ -17525,7 +17709,7 @@
     <row r="24" ht="24" customHeight="1" spans="3:15">
       <c r="C24" s="34"/>
       <c r="D24" s="50" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="E24" s="36"/>
       <c r="F24" s="37">
@@ -17560,7 +17744,7 @@
     <row r="25" ht="24" customHeight="1" spans="3:15">
       <c r="C25" s="34"/>
       <c r="D25" s="50" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="E25" s="36"/>
       <c r="F25" s="37">
@@ -17595,7 +17779,7 @@
     <row r="26" ht="24" customHeight="1" spans="3:15">
       <c r="C26" s="34"/>
       <c r="D26" s="50" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="E26" s="36"/>
       <c r="F26" s="37">
@@ -17630,7 +17814,7 @@
     <row r="27" ht="24" customHeight="1" spans="3:15">
       <c r="C27" s="34"/>
       <c r="D27" s="50" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="37">
@@ -17665,7 +17849,7 @@
     <row r="28" ht="24" customHeight="1" spans="3:15">
       <c r="C28" s="34"/>
       <c r="D28" s="50" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="E28" s="36"/>
       <c r="F28" s="37">
@@ -17700,7 +17884,7 @@
     <row r="29" ht="24" customHeight="1" spans="3:15">
       <c r="C29" s="34"/>
       <c r="D29" s="50" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="E29" s="36"/>
       <c r="F29" s="37">
@@ -17776,7 +17960,7 @@
     <row r="31" ht="24" customHeight="1" spans="3:15">
       <c r="C31" s="34"/>
       <c r="D31" s="50" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="E31" s="36"/>
       <c r="F31" s="37">
@@ -17811,7 +17995,7 @@
     <row r="32" ht="24" customHeight="1" spans="3:15">
       <c r="C32" s="34"/>
       <c r="D32" s="50" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="E32" s="36"/>
       <c r="F32" s="37">
@@ -17846,7 +18030,7 @@
     <row r="33" ht="24" customHeight="1" spans="3:15">
       <c r="C33" s="34"/>
       <c r="D33" s="50" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="E33" s="36"/>
       <c r="F33" s="37">
@@ -17881,7 +18065,7 @@
     <row r="34" ht="24" customHeight="1" spans="3:15">
       <c r="C34" s="34"/>
       <c r="D34" s="50" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="E34" s="36"/>
       <c r="F34" s="37">
@@ -17916,7 +18100,7 @@
     <row r="35" ht="24" customHeight="1" spans="3:15">
       <c r="C35" s="34"/>
       <c r="D35" s="50" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="E35" s="36"/>
       <c r="F35" s="37">
@@ -17951,7 +18135,7 @@
     <row r="36" ht="24" customHeight="1" spans="3:15">
       <c r="C36" s="34"/>
       <c r="D36" s="50" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="E36" s="36"/>
       <c r="F36" s="37">
@@ -17986,7 +18170,7 @@
     <row r="37" ht="24" customHeight="1" spans="3:15">
       <c r="C37" s="34"/>
       <c r="D37" s="50" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="E37" s="36"/>
       <c r="F37" s="37">
@@ -18062,7 +18246,7 @@
     <row r="39" ht="24" customHeight="1" spans="3:15">
       <c r="C39" s="34"/>
       <c r="D39" s="50" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="E39" s="56"/>
       <c r="F39" s="37">
@@ -18097,7 +18281,7 @@
     <row r="40" ht="24" customHeight="1" spans="3:15">
       <c r="C40" s="34"/>
       <c r="D40" s="50" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="E40" s="36"/>
       <c r="F40" s="37">
@@ -18132,7 +18316,7 @@
     <row r="41" ht="24" customHeight="1" spans="3:15">
       <c r="C41" s="34"/>
       <c r="D41" s="50" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="E41" s="36"/>
       <c r="F41" s="37">
@@ -18890,7 +19074,7 @@
       <c r="B60" s="54"/>
       <c r="C60" s="60"/>
       <c r="D60" s="45" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="E60" s="61"/>
       <c r="F60" s="47">
@@ -19006,7 +19190,7 @@
       <c r="B63" s="54"/>
       <c r="C63" s="60"/>
       <c r="D63" s="45" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="E63" s="61"/>
       <c r="F63" s="47">
@@ -19242,7 +19426,7 @@
       <c r="B69" s="54"/>
       <c r="C69" s="60"/>
       <c r="D69" s="45" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="E69" s="61"/>
       <c r="F69" s="47">
@@ -19398,7 +19582,7 @@
       <c r="B73" s="54"/>
       <c r="C73" s="60"/>
       <c r="D73" s="45" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="E73" s="61"/>
       <c r="F73" s="47">
@@ -19525,7 +19709,7 @@
     </row>
     <row r="77" spans="14:14">
       <c r="N77" s="89" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>